<commit_message>
modifying mapping and updating schema imports
</commit_message>
<xml_diff>
--- a/shared/ojb-resources-common/src/main/resources/service-specifications/ECF_Court_Filing_Service/artifacts/service_model/information_model/ECF_Court_Filing_IEPD/documentation/impl-artifacts/vermont/Citation_Case_Mapping.xlsx
+++ b/shared/ojb-resources-common/src/main/resources/service-specifications/ECF_Court_Filing_Service/artifacts/service_model/information_model/ECF_Court_Filing_IEPD/documentation/impl-artifacts/vermont/Citation_Case_Mapping.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26221"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25306"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="5260" yWindow="2780" windowWidth="29840" windowHeight="15880"/>
+    <workbookView xWindow="6000" yWindow="880" windowWidth="20880" windowHeight="15880"/>
   </bookViews>
   <sheets>
     <sheet name="eCitation" sheetId="1" r:id="rId1"/>
@@ -649,229 +649,7 @@
 (Elements in RED are OJB extensions to ECF)</t>
   </si>
   <si>
-    <t>/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ojb-cit-ext:Citation/nc:ActivityIdentification/nc:IdentificationID</t>
-  </si>
-  <si>
-    <t>/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ojb-cit-ext:Citation/nc:ActivityDate/nc:Date</t>
-  </si>
-  <si>
-    <t>/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ojb-cit-ext:Citation/ojb-cit-ext:CitationAugmentation/ojb-cit-ext:CitationWaiverAmount</t>
-  </si>
-  <si>
-    <t>/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ojb-cit-ext:Citation/ojb-cit-ext:CitationAugmentation/ojb-cit-ext:CitationServedIndicator</t>
-  </si>
-  <si>
-    <t>/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ojb-cit-ext:Citation/ojb-cit-ext:CitationAugmentation/ojb-cit-ext:CitationMailedIndicator</t>
-  </si>
-  <si>
-    <t>/ojb-cit-doc:CitationCase/ojb-cit-ext:CaseAugmentation/ojb-cit-ext:CaseParticipant/ecf:EntityOrganization/nc:OrganizationName</t>
-  </si>
-  <si>
-    <t>/ojb-cit-doc:CitationCase/ojb-cit-ext:CaseAugmentation/ojb-cit-ext:CaseParticipant/ecf:EntityOrganization[@s:id=/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationDeliveryRecipientAssociation/nc:EntityOrganizationReference/@s:ref]/nc:OrganizationName</t>
-  </si>
-  <si>
-    <t>/ojb-cit-doc:CitationCase/ojb-cit-ext:CaseAugmentation/ojb-cit-ext:CaseParticipant/ojb-cit-ext:EntityPerson[@s:id=/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ecf-cit:CitationSubject/nc:RoleOfPersonReference/@s:ref]/nc:PersonName/nc:PersonSurName</t>
-  </si>
-  <si>
-    <t>/ojb-cit-doc:CitationCase/ojb-cit-ext:CaseAugmentation/ojb-cit-ext:CaseParticipant/ojb-cit-ext:EntityPerson[@s:id=/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ecf-cit:CitationSubject/nc:RoleOfPersonReference/@s:ref]/nc:PersonName/nc:PersonGivenName</t>
-  </si>
-  <si>
-    <t>/ojb-cit-doc:CitationCase/ojb-cit-ext:CaseAugmentation/ojb-cit-ext:CaseParticipant/ojb-cit-ext:EntityPerson[@s:id=/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ecf-cit:CitationSubject/nc:RoleOfPersonReference/@s:ref]/nc:PersonName/nc:PersonMiddleName</t>
-  </si>
-  <si>
-    <t>/ojb-cit-doc:CitationCase/ojb-cit-ext:CaseAugmentation/ojb-cit-ext:CaseParticipant/ojb-cit-ext:EntityPerson[@s:id=/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ecf-cit:CitationSubject/nc:RoleOfPersonReference/@s:ref]/nc:PersonBirthLocation/nc:LocationAddress/nc:StructuredAddress/nc:LocationCityName</t>
-  </si>
-  <si>
-    <t>/ojb-cit-doc:CitationCase/ojb-cit-ext:CaseAugmentation/ojb-cit-ext:CaseParticipant/ojb-cit-ext:EntityPerson[@s:id=/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ecf-cit:CitationSubject/nc:RoleOfPersonReference/@s:ref]/nc:PersonSexCode</t>
-  </si>
-  <si>
-    <t>/ojb-cit-doc:CitationCase/ojb-cit-ext:CaseAugmentation/ojb-cit-ext:CaseParticipant/ojb-cit-ext:EntityPerson[@s:id=/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ecf-cit:CitationSubject/nc:RoleOfPersonReference/@s:ref]/nc:PersonBirthDate/nc:Date</t>
-  </si>
-  <si>
-    <t>/ojb-cit-doc:CitationCase/ojb-cit-ext:CaseAugmentation/ojb-cit-ext:CaseParticipant/ojb-cit-ext:EntityPerson[@s:id=/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ecf-cit:CitationSubject/nc:RoleOfPersonReference/@s:ref]/nc:PersonHeightMeasure/nc:MeasureText</t>
-  </si>
-  <si>
-    <t>/ojb-cit-doc:CitationCase/ojb-cit-ext:CaseAugmentation/ojb-cit-ext:CaseParticipant/ojb-cit-ext:EntityPerson[@s:id=/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ecf-cit:CitationSubject/nc:RoleOfPersonReference/@s:ref]/nc:PersonHeightMeasure/nc:MeasureUnitText</t>
-  </si>
-  <si>
-    <t>/ojb-cit-doc:CitationCase/ojb-cit-ext:CaseAugmentation/ojb-cit-ext:CaseParticipant/ojb-cit-ext:EntityPerson[@s:id=/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ecf-cit:CitationSubject/nc:RoleOfPersonReference/@s:ref]/nc:PersonWeightMeasure/nc:MeasureUnitText</t>
-  </si>
-  <si>
-    <t>/ojb-cit-doc:CitationCase/ojb-cit-ext:CaseAugmentation/ojb-cit-ext:CaseParticipant/ojb-cit-ext:EntityPerson[@s:id=/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ecf-cit:CitationSubject/nc:RoleOfPersonReference/@s:ref]/nc:PersonWeightMeasure/nc:MeasureText</t>
-  </si>
-  <si>
-    <t>/ojb-cit-doc:CitationCase/ojb-cit-ext:CaseAugmentation/ojb-cit-ext:CaseParticipant/ojb-cit-ext:EntityPerson[@s:id=/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ecf-cit:CitationSubject/nc:RoleOfPersonReference/@s:ref]/nc:PersonHairColorCode</t>
-  </si>
-  <si>
-    <t>/ojb-cit-doc:CitationCase/ojb-cit-ext:CaseAugmentation/ojb-cit-ext:CaseParticipant/ojb-cit-ext:EntityPerson[@s:id=/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ecf-cit:CitationSubject/nc:RoleOfPersonReference/@s:ref]/nc:PersonEyeColorCode</t>
-  </si>
-  <si>
-    <t>/ojb-cit-doc:CitationCase/ojb-cit-ext:CaseAugmentation/ojb-cit-ext:CaseParticipant/ojb-cit-ext:EntityPerson[@s:id=/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ecf-cit:CitationSubject/nc:RoleOfPersonReference/@s:ref]/ojb-cit-ext:PersonAugmentation/ojb-cit-ext:PersonDriverLicense/nc:DriverLicenseIdentification/nc:IdentificationID</t>
-  </si>
-  <si>
-    <t>/ojb-cit-doc:CitationCase/ojb-cit-ext:CaseAugmentation/ojb-cit-ext:CaseParticipant/ojb-cit-ext:EntityPerson[@s:id=/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ecf-cit:CitationSubject/nc:RoleOfPersonReference/@s:ref]/ojb-cit-ext:PersonAugmentation/nc:ContactInformation/nc:ContactMailingAddress/nc:StructuredAddress/nc:LocationPostalCode</t>
-  </si>
-  <si>
-    <t>/ojb-cit-doc:CitationCase/ojb-cit-ext:CaseAugmentation/ojb-cit-ext:CaseParticipant/ojb-cit-ext:EntityPerson[@s:id=/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ecf-cit:CitationSubject/nc:RoleOfPersonReference/@s:ref]/ojb-cit-ext:PersonAugmentation/nc:ContactInformation/nc:ContactMailingAddress/nc:StructuredAddress/nc:LocationStreet/nc:StreetFullText</t>
-  </si>
-  <si>
-    <t>/ojb-cit-doc:CitationCase/ojb-cit-ext:CaseAugmentation/ojb-cit-ext:CaseParticipant/ojb-cit-ext:EntityPerson[@s:id=/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ecf-cit:CitationSubject/nc:RoleOfPersonReference/@s:ref]/ojb-cit-ext:PersonAugmentation/nc:ContactInformation/nc:ContactMailingAddress/nc:StructuredAddress/nc:LocationCityName</t>
-  </si>
-  <si>
-    <t>/ojb-cit-doc:CitationCase/ojb-cit-ext:CaseAugmentation/ojb-cit-ext:CaseParticipant/ojb-cit-ext:EntityPerson[@s:id=/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ecf-cit:CitationSubject/nc:RoleOfPersonReference/@s:ref]/ojb-cit-ext:PersonAugmentation/nc:ContactInformation/nc:ContactMailingAddress/nc:StructuredAddress/nc:LocationCountryFIPS10-4Code</t>
-  </si>
-  <si>
-    <t>/ojb-cit-doc:CitationCase/ojb-cit-ext:CaseAugmentation/ojb-cit-ext:CaseParticipant/ojb-cit-ext:EntityPerson[@s:id=/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ecf-cit:CitationSubject/nc:RoleOfPersonReference/@s:ref]/ojb-cit-ext:PersonAugmentation/ojb-cit-ext:PersonDriverLicense/nc:DriverLicenseIdentification/j:IdentificationJurisdictionNCICLISCode</t>
-  </si>
-  <si>
-    <t>/ojb-cit-doc:CitationCase/ojb-cit-ext:CaseAugmentation/ojb-cit-ext:CaseParticipant/ojb-cit-ext:EntityPerson[@s:id=/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ecf-cit:CitationSubject/nc:RoleOfPersonReference/@s:ref]/ojb-cit-ext:PersonAugmentation/ojb-cit-ext:PersonDriverLicense/ojb-cit-ext:DriverLicenseCDLIndicator</t>
-  </si>
-  <si>
-    <t>/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ojb-cit-ext:Vehicle[@s:id=/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ojb-cit-ext:DrivingIncident/nc:IncidentVehicleAssociation/nc:ConveyanceReference/@s:ref]/nc:VehicleIdentification/nc:IdentificationID</t>
-  </si>
-  <si>
-    <t>/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ojb-cit-ext:Vehicle[@s:id=/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ojb-cit-ext:DrivingIncident/nc:IncidentVehicleAssociation/nc:ConveyanceReference/@s:ref]/nc:ConveyanceRegistrationPlateIdentification/nc:IdentificationID</t>
-  </si>
-  <si>
-    <t>/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ojb-cit-ext:Vehicle[@s:id=/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ojb-cit-ext:DrivingIncident/nc:IncidentVehicleAssociation/nc:ConveyanceReference/@s:ref]/nc:ConveyanceRegistrationPlateIdentification/j:IdentificationJurisdictionNCICLISCode</t>
-  </si>
-  <si>
-    <t>/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ojb-cit-ext:Vehicle[@s:id=/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ojb-cit-ext:DrivingIncident/nc:IncidentVehicleAssociation/nc:ConveyanceReference/@s:ref]/nc:ItemModelYearDate</t>
-  </si>
-  <si>
-    <t>/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ojb-cit-ext:Vehicle[@s:id=/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ojb-cit-ext:DrivingIncident/nc:IncidentVehicleAssociation/nc:ConveyanceReference/@s:ref]/nc:VehicleMakeCode</t>
-  </si>
-  <si>
-    <t>/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ojb-cit-ext:Vehicle[@s:id=/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ojb-cit-ext:DrivingIncident/nc:IncidentVehicleAssociation/nc:ConveyanceReference/@s:ref]/nc:VehicleColorPrimaryCode</t>
-  </si>
-  <si>
-    <t>/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ojb-cit-ext:Vehicle[@s:id=/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ojb-cit-ext:DrivingIncident/nc:IncidentVehicleAssociation/nc:ConveyanceReference/@s:ref]/nc:VehicleStyleCode</t>
-  </si>
-  <si>
-    <t>/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ojb-cit-ext:Vehicle[@s:id=/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ojb-cit-ext:DrivingIncident/nc:IncidentVehicleAssociation/nc:ConveyanceReference/@s:ref]/nc:VehicleCMVIndicator</t>
-  </si>
-  <si>
-    <t>/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ojb-cit-ext:Vehicle[@s:id=/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ojb-cit-ext:DrivingIncident/nc:IncidentVehicleAssociation/nc:ConveyanceReference/@s:ref]/ojb-cit-ext:VehicleAugmentation/ojb-cit-ext:VehicleHazardousMaterialIndicator</t>
-  </si>
-  <si>
-    <t>/ojb-cit-doc:CitationCase/ojb-cit-ext:CaseAugmentation/ojb-cit-ext:CaseParticipant/ojb-cit-ext:EntityPerson[@s:id=/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ecf-cit:CitationSubject/nc:RoleOfPersonReference/@s:ref]//ojb-cit-ext:PersonAugmentation/ojb-cit-ext:PersonFishAndWildlifeLicenseIdentification/nc:IdentificationID</t>
-  </si>
-  <si>
-    <t>/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ojb-cit-ext:DrivingIncident[@s:id=/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ojb-cit-ext:DrivingIncident/nc:IncidentVehicleAssociation/nc:ActivityReference/@s:ref]/nc:ActivityIdentification/nc:IdentificationID</t>
-  </si>
-  <si>
-    <t>/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ojb-cit-ext:DrivingIncident[@s:id=/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ojb-cit-ext:DrivingIncident/nc:IncidentVehicleAssociation/nc:ActivityReference/@s:ref]/nc:ActivityDate/nc:DateTime</t>
-  </si>
-  <si>
-    <t>/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ojb-cit-ext:DrivingIncident[@s:id=/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ojb-cit-ext:DrivingIncident/nc:IncidentVehicleAssociation/nc:ActivityReference/@s:ref]/nc:IncidentLocation/nc:LocationAddress/nc:StructuredAddress/nc:LocationCityName</t>
-  </si>
-  <si>
-    <t>/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ojb-cit-ext:DrivingIncident[@s:id=/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ojb-cit-ext:DrivingIncident/nc:IncidentVehicleAssociation/nc:ActivityReference/@s:ref]/nc:IncidentLocation/nc:LocationHighway/nc:HighwayID</t>
-  </si>
-  <si>
-    <t>/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ojb-cit-ext:DrivingIncident[@s:id=/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ojb-cit-ext:DrivingIncident/nc:IncidentVehicleAssociation/nc:ActivityReference/@s:ref]/nc:IncidentLocation/nc:LocationHighway/nc:HighwayPositionText</t>
-  </si>
-  <si>
-    <t>/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ojb-cit-ext:DrivingIncident[@s:id=/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ojb-cit-ext:DrivingIncident/nc:IncidentVehicleAssociation/nc:ActivityReference/@s:ref]/nc:ActivityDescriptionText</t>
-  </si>
-  <si>
-    <t>/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ecf-cit:CitationSubject/ecf-cit:PersonBloodAlcoholNumber</t>
-  </si>
-  <si>
-    <t>/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ojb-cit-ext:DrivingIncident[@s:id=/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ojb-cit-ext:DrivingIncident/nc:IncidentVehicleAssociation/nc:ActivityReference/@s:ref]/j:DrivingIncidentRecordedSpeedRate/nc:MeasureText</t>
-  </si>
-  <si>
-    <t>/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ojb-cit-ext:DrivingIncident[@s:id=/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ojb-cit-ext:DrivingIncident/nc:IncidentVehicleAssociation/nc:ActivityReference/@s:ref]/j:DrivingIncidentRecordedSpeedRate/nc:MeasureUnitText</t>
-  </si>
-  <si>
-    <t>/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ojb-cit-ext:DrivingIncident[@s:id=/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ojb-cit-ext:DrivingIncident/nc:IncidentVehicleAssociation/nc:ActivityReference/@s:ref]/j:DrivingIncidentLegalSpeedRate/nc:MeasureText</t>
-  </si>
-  <si>
-    <t>/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ojb-cit-ext:DrivingIncident[@s:id=/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ojb-cit-ext:DrivingIncident/nc:IncidentVehicleAssociation/nc:ActivityReference/@s:ref]/j:DrivingIncidentLegalSpeedRate/nc:MeasureUnitText</t>
-  </si>
-  <si>
-    <t>/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ojb-cit-ext:DrivingIncident[@s:id=/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ojb-cit-ext:DrivingIncident/nc:IncidentVehicleAssociation/nc:ActivityReference/@s:ref]/ojb-cit-ext:DrivingIncidentAugmentation/ojb-cit-ext:DrivingAccidentFatalityIndicator</t>
-  </si>
-  <si>
-    <t>/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ojb-cit-ext:DrivingIncident[@s:id=/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ojb-cit-ext:DrivingIncident/nc:IncidentVehicleAssociation/nc:ActivityReference/@s:ref]/j:IncidentAugmentation/j:IncidentTrafficAccidentInvolvedIndicator</t>
-  </si>
-  <si>
-    <t>/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ojb-cit-ext:DrivingIncident[@s:id=/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ojb-cit-ext:DrivingIncident/nc:IncidentVehicleAssociation/nc:ActivityReference/@s:ref]/ojb-cit-ext:DrivingIncidentAugmentation/ojb-cit-ext:SeatBeltViolationIndicator</t>
-  </si>
-  <si>
-    <t>/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ojb-cit-ext:DrivingIncident[@s:id=/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ojb-cit-ext:DrivingIncident/nc:IncidentVehicleAssociation/nc:ActivityReference/@s:ref]/ojb-cit-ext:DrivingIncidentAugmentation/ojb-cit-ext:CityReliefActIndicator</t>
-  </si>
-  <si>
-    <t>/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ojb-cit-ext:DrivingIncident[@s:id=/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ojb-cit-ext:DrivingIncident/nc:IncidentVehicleAssociation/nc:ActivityReference/@s:ref]/ojb-cit-ext:DrivingIncidentAugmentation/ojb-cit-ext:CityReliefActJuvenileIndicator</t>
-  </si>
-  <si>
-    <t>/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ojb-cit-ext:DrivingIncident[@s:id=/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ojb-cit-ext:DrivingIncident/nc:IncidentVehicleAssociation/nc:ActivityReference/@s:ref]/ojb-cit-ext:DrivingIncidentAugmentation/ojb-cit-ext:CityReliefActOtherIndicator</t>
-  </si>
-  <si>
-    <t>/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ojb-cit-ext:DrivingIncident[@s:id=/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ojb-cit-ext:DrivingIncident/nc:IncidentVehicleAssociation/nc:ActivityReference/@s:ref]/ojb-cit-ext:DrivingIncidentAugmentation/ojb-cit-ext:CityReliefActOtherText</t>
-  </si>
-  <si>
-    <t>/ojb-cit-doc:CitationCase/ojb-cit-ext:CaseAugmentation/ojb-cit-ext:CaseParticipant/ecf:EntityPerson[@s:id=/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ojb-cit-ext:Citation/j:CitationIssuingOfficial/nc:RoleOfPersonReference/@s:ref]/nc:PersonName/nc:PersonFullName</t>
-  </si>
-  <si>
     <t>N/A</t>
-  </si>
-  <si>
-    <t>/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ojb-cit-ext:Citation/j:CitationIssuingOfficial/j:EnforcementOfficialBadgeIdentification/nc:IdentificationID</t>
-  </si>
-  <si>
-    <t>/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ojb-cit-ext:Citation/j:CitationAgency/nc:OrganizationName</t>
-  </si>
-  <si>
-    <t>/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ojb-cit-ext:Citation/j:CitationAgency/nc:OrganizationPrimaryContactInformation/nc:ContactEntity/ecf:EntityOrganization/j:OrganizationAugmentation/j:OrganizationORIIdentification/nc:IdentificationID</t>
-  </si>
-  <si>
-    <t>/ojb-cit-doc:CitationCase/ojb-cit-ext:CaseAugmentation/ojb-cit-ext:CaseParticipant/ecf:EntityPerson[@s:id=/ojb-cit-doc:CitationCase/nc:ImmediateFamilyAssociation/nc:PersonParentReference/@s:ref]/nc:PersonName/nc:PersonGivenName</t>
-  </si>
-  <si>
-    <t>/ojb-cit-doc:CitationCase/ojb-cit-ext:CaseAugmentation/ojb-cit-ext:CaseParticipant/ecf:EntityPerson[@s:id=/ojb-cit-doc:CitationCase/nc:ImmediateFamilyAssociation/nc:PersonParentReference/@s:ref]/nc:PersonName/nc:PersonSurName</t>
-  </si>
-  <si>
-    <t>/ojb-cit-doc:CitationCase/ojb-cit-ext:CaseAugmentation/ojb-cit-ext:CaseParticipant/ecf:EntityPerson[@s:id=/ojb-cit-doc:CitationCase/nc:ImmediateFamilyAssociation/nc:PersonParentReference/@s:ref]/ecf:PersonAugmentation/nc:ContactInformation/nc:ContactMailingAddress/nc:StructuredAddress/nc:LocationStreet/nc:StreetFullText</t>
-  </si>
-  <si>
-    <t>/ojb-cit-doc:CitationCase/ojb-cit-ext:CaseAugmentation/ojb-cit-ext:CaseParticipant/ecf:EntityPerson[@s:id=/ojb-cit-doc:CitationCase/nc:ImmediateFamilyAssociation/nc:PersonParentReference/@s:ref]/ecf:PersonAugmentation/nc:ContactInformation/nc:ContactMailingAddress/nc:StructuredAddress/nc:LocationCityName</t>
-  </si>
-  <si>
-    <t>/ojb-cit-doc:CitationCase/ojb-cit-ext:CaseAugmentation/ojb-cit-ext:CaseParticipant/ecf:EntityPerson[@s:id=/ojb-cit-doc:CitationCase/nc:ImmediateFamilyAssociation/nc:PersonParentReference/@s:ref]/ecf:PersonAugmentation/nc:ContactInformation/nc:ContactMailingAddress/nc:StructuredAddress/nc:LocationCountryFIPS10-4Code</t>
-  </si>
-  <si>
-    <t>/ojb-cit-doc:CitationCase/ojb-cit-ext:CaseAugmentation/ojb-cit-ext:CaseParticipant/ecf:EntityPerson[@s:id=/ojb-cit-doc:CitationCase/nc:ImmediateFamilyAssociation/nc:PersonParentReference/@s:ref]/ecf:PersonAugmentation/nc:ContactInformation/nc:ContactMailingAddress/nc:StructuredAddress/nc:LocationPostalCode</t>
-  </si>
-  <si>
-    <t>/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ojb-cit-ext:Offense/j:Statute/j:StatuteCodeIdentification/nc:IdentificationID</t>
-  </si>
-  <si>
-    <t>/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ojb-cit-ext:Offense/ojb-cit-ext:OffenseViolatedStatute/j:StatuteCodeIdentification/nc:IdentificationID</t>
-  </si>
-  <si>
-    <t>/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ojb-cit-ext:Offense/ojb-cit-ext:CFRStatute/j:StatuteCodeIdentification/nc:IdentificationID</t>
-  </si>
-  <si>
-    <t>/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/j:CaseCharge/j:ChargeStatute/j:StatuteOffenseIdentification/nc:IdentificationID</t>
-  </si>
-  <si>
-    <t>/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ojb-cit-ext:Offense/ojb-cit-ext:RelatedCriminalChargeIndicator</t>
-  </si>
-  <si>
-    <t>/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ojb-cit-ext:Offense/ojb-cit-ext:DrivingOffensePoints</t>
-  </si>
-  <si>
-    <t>/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ojb-cit-ext:Offense/ojb-cit-ext:OffenseFineAmountMinimum</t>
-  </si>
-  <si>
-    <t>/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ojb-cit-ext:Offense/ojb-cit-ext:OffenseFineAmountMaximum</t>
-  </si>
-  <si>
-    <t>/ojb-cit-doc:CitationCase/ojb-cit-ext:CaseAugmentation/ojb-cit-ext:CaseParticipant/ojb-cit-ext:EntityPerson[@s:id=/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ecf-cit:CitationSubject/nc:RoleOfPersonReference/@s:ref]/ojb-cit-ext:PersonAugmentation/nc:ContactInformation/nc:ContactTelephoneNumber[@s:id=/ojb-cit-doc:CitationCase/ojb-cit-ext:CaseAugmentation/ojb-cit-ext:CaseParticipant/ojb-cit-ext:EntityPerson/ojb-cit-ext:PersonAugmentation/nc:PersonContactInformationAssociation[nc:ContactInformationIsHomeIndicator="true"]/nc:ContactInformationReference/@s:ref]/nc:FullTelephoneNumber/nc:TelephoneNumberFullID</t>
-  </si>
-  <si>
-    <t>/ojb-cit-doc:CitationCase/ojb-cit-ext:CaseAugmentation/ojb-cit-ext:CaseParticipant/ojb-cit-ext:EntityPerson[@s:id=/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ecf-cit:CitationSubject/nc:RoleOfPersonReference/@s:ref]/ojb-cit-ext:PersonAugmentation/nc:ContactInformation/nc:ContactTelephoneNumber[@s:id=/ojb-cit-doc:CitationCase/ojb-cit-ext:CaseAugmentation/ojb-cit-ext:CaseParticipant/ojb-cit-ext:EntityPerson/ojb-cit-ext:PersonAugmentation/nc:PersonContactInformationAssociation[nc:ContactInformationIsWorkIndicator="true"]/nc:ContactInformationReference/@s:ref]/nc:FullTelephoneNumber/nc:TelephoneNumberFullID</t>
   </si>
   <si>
     <t>ECF Mapping</t>
@@ -879,6 +657,228 @@
   <si>
     <t>Highlighted elements are not in the ECF NIEM subset
 ECF extension elements are in red.</t>
+  </si>
+  <si>
+    <t>/ecf-cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ojb-cit-ext:Citation/nc:ActivityIdentification/nc:IdentificationID</t>
+  </si>
+  <si>
+    <t>/ecf-cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ojb-cit-ext:Citation/nc:ActivityDate/nc:Date</t>
+  </si>
+  <si>
+    <t>/ecf-cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ojb-cit-ext:Citation/ojb-cit-ext:CitationAugmentation/ojb-cit-ext:CitationWaiverAmount</t>
+  </si>
+  <si>
+    <t>/ecf-cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ojb-cit-ext:Citation/ojb-cit-ext:CitationAugmentation/ojb-cit-ext:CitationServedIndicator</t>
+  </si>
+  <si>
+    <t>/ecf-cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ojb-cit-ext:Citation/ojb-cit-ext:CitationAugmentation/ojb-cit-ext:CitationMailedIndicator</t>
+  </si>
+  <si>
+    <t>/ecf-cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CaseAugmentation/ojb-cit-ext:CaseParticipant/ecf:EntityOrganization/nc:OrganizationName</t>
+  </si>
+  <si>
+    <t>/ecf-cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CaseAugmentation/ojb-cit-ext:CaseParticipant/ecf:EntityOrganization[@s:id=/ecf-cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationDeliveryRecipientAssociation/nc:EntityOrganizationReference/@s:ref]/nc:OrganizationName</t>
+  </si>
+  <si>
+    <t>/ecf-cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CaseAugmentation/ojb-cit-ext:CaseParticipant/ojb-cit-ext:EntityPerson[@s:id=/ecf-cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ecf-cit:CitationSubject/nc:RoleOfPersonReference/@s:ref]/nc:PersonName/nc:PersonSurName</t>
+  </si>
+  <si>
+    <t>/ecf-cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CaseAugmentation/ojb-cit-ext:CaseParticipant/ojb-cit-ext:EntityPerson[@s:id=/ecf-cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ecf-cit:CitationSubject/nc:RoleOfPersonReference/@s:ref]/nc:PersonName/nc:PersonGivenName</t>
+  </si>
+  <si>
+    <t>/ecf-cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CaseAugmentation/ojb-cit-ext:CaseParticipant/ojb-cit-ext:EntityPerson[@s:id=/ecf-cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ecf-cit:CitationSubject/nc:RoleOfPersonReference/@s:ref]/nc:PersonName/nc:PersonMiddleName</t>
+  </si>
+  <si>
+    <t>/ecf-cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CaseAugmentation/ojb-cit-ext:CaseParticipant/ojb-cit-ext:EntityPerson[@s:id=/ecf-cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ecf-cit:CitationSubject/nc:RoleOfPersonReference/@s:ref]/ojb-cit-ext:PersonAugmentation/nc:ContactInformation/nc:ContactMailingAddress/nc:StructuredAddress/nc:LocationStreet/nc:StreetFullText</t>
+  </si>
+  <si>
+    <t>/ecf-cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CaseAugmentation/ojb-cit-ext:CaseParticipant/ojb-cit-ext:EntityPerson[@s:id=/ecf-cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ecf-cit:CitationSubject/nc:RoleOfPersonReference/@s:ref]/ojb-cit-ext:PersonAugmentation/nc:ContactInformation/nc:ContactMailingAddress/nc:StructuredAddress/nc:LocationCityName</t>
+  </si>
+  <si>
+    <t>/ecf-cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CaseAugmentation/ojb-cit-ext:CaseParticipant/ojb-cit-ext:EntityPerson[@s:id=/ecf-cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ecf-cit:CitationSubject/nc:RoleOfPersonReference/@s:ref]/ojb-cit-ext:PersonAugmentation/nc:ContactInformation/nc:ContactMailingAddress/nc:StructuredAddress/nc:LocationCountryFIPS10-4Code</t>
+  </si>
+  <si>
+    <t>/ecf-cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CaseAugmentation/ojb-cit-ext:CaseParticipant/ojb-cit-ext:EntityPerson[@s:id=/ecf-cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ecf-cit:CitationSubject/nc:RoleOfPersonReference/@s:ref]/ojb-cit-ext:PersonAugmentation/nc:ContactInformation/nc:ContactMailingAddress/nc:StructuredAddress/nc:LocationPostalCode</t>
+  </si>
+  <si>
+    <t>/ecf-cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CaseAugmentation/ojb-cit-ext:CaseParticipant/ojb-cit-ext:EntityPerson[@s:id=/ecf-cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ecf-cit:CitationSubject/nc:RoleOfPersonReference/@s:ref]/ojb-cit-ext:PersonAugmentation/ojb-cit-ext:PersonDriverLicense/nc:DriverLicenseIdentification/nc:IdentificationID</t>
+  </si>
+  <si>
+    <t>/ecf-cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CaseAugmentation/ojb-cit-ext:CaseParticipant/ojb-cit-ext:EntityPerson[@s:id=/ecf-cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ecf-cit:CitationSubject/nc:RoleOfPersonReference/@s:ref]/ojb-cit-ext:PersonAugmentation/ojb-cit-ext:PersonDriverLicense/nc:DriverLicenseIdentification/j:IdentificationJurisdictionNCICLISCode</t>
+  </si>
+  <si>
+    <t>/ecf-cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CaseAugmentation/ojb-cit-ext:CaseParticipant/ojb-cit-ext:EntityPerson[@s:id=/ecf-cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ecf-cit:CitationSubject/nc:RoleOfPersonReference/@s:ref]//ojb-cit-ext:PersonAugmentation/ojb-cit-ext:PersonFishAndWildlifeLicenseIdentification/nc:IdentificationID</t>
+  </si>
+  <si>
+    <t>/ecf-cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CaseAugmentation/ojb-cit-ext:CaseParticipant/ojb-cit-ext:EntityPerson[@s:id=/ecf-cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ecf-cit:CitationSubject/nc:RoleOfPersonReference/@s:ref]/ojb-cit-ext:PersonAugmentation/nc:ContactInformation/nc:ContactTelephoneNumber[@s:id=/ecf-cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CaseAugmentation/ojb-cit-ext:CaseParticipant/ojb-cit-ext:EntityPerson/ojb-cit-ext:PersonAugmentation/nc:PersonContactInformationAssociation[nc:ContactInformationIsHomeIndicator="true"]/nc:ContactInformationReference/@s:ref]/nc:FullTelephoneNumber/nc:TelephoneNumberFullID</t>
+  </si>
+  <si>
+    <t>/ecf-cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CaseAugmentation/ojb-cit-ext:CaseParticipant/ojb-cit-ext:EntityPerson[@s:id=/ecf-cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ecf-cit:CitationSubject/nc:RoleOfPersonReference/@s:ref]/ojb-cit-ext:PersonAugmentation/nc:ContactInformation/nc:ContactTelephoneNumber[@s:id=/ecf-cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CaseAugmentation/ojb-cit-ext:CaseParticipant/ojb-cit-ext:EntityPerson/ojb-cit-ext:PersonAugmentation/nc:PersonContactInformationAssociation[nc:ContactInformationIsWorkIndicator="true"]/nc:ContactInformationReference/@s:ref]/nc:FullTelephoneNumber/nc:TelephoneNumberFullID</t>
+  </si>
+  <si>
+    <t>/ecf-cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CaseAugmentation/ojb-cit-ext:CaseParticipant/ojb-cit-ext:EntityPerson[@s:id=/ecf-cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ecf-cit:CitationSubject/nc:RoleOfPersonReference/@s:ref]/nc:PersonBirthDate/nc:Date</t>
+  </si>
+  <si>
+    <t>/ecf-cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CaseAugmentation/ojb-cit-ext:CaseParticipant/ojb-cit-ext:EntityPerson[@s:id=/ecf-cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ecf-cit:CitationSubject/nc:RoleOfPersonReference/@s:ref]/nc:PersonSexCode</t>
+  </si>
+  <si>
+    <t>/ecf-cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CaseAugmentation/ojb-cit-ext:CaseParticipant/ojb-cit-ext:EntityPerson[@s:id=/ecf-cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ecf-cit:CitationSubject/nc:RoleOfPersonReference/@s:ref]/nc:PersonBirthLocation/nc:LocationAddress/nc:StructuredAddress/nc:LocationCityName</t>
+  </si>
+  <si>
+    <t>/ecf-cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CaseAugmentation/ojb-cit-ext:CaseParticipant/ojb-cit-ext:EntityPerson[@s:id=/ecf-cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ecf-cit:CitationSubject/nc:RoleOfPersonReference/@s:ref]/nc:PersonHeightMeasure/nc:MeasureText</t>
+  </si>
+  <si>
+    <t>/ecf-cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CaseAugmentation/ojb-cit-ext:CaseParticipant/ojb-cit-ext:EntityPerson[@s:id=/ecf-cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ecf-cit:CitationSubject/nc:RoleOfPersonReference/@s:ref]/nc:PersonHeightMeasure/nc:MeasureUnitText</t>
+  </si>
+  <si>
+    <t>/ecf-cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CaseAugmentation/ojb-cit-ext:CaseParticipant/ojb-cit-ext:EntityPerson[@s:id=/ecf-cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ecf-cit:CitationSubject/nc:RoleOfPersonReference/@s:ref]/nc:PersonWeightMeasure/nc:MeasureText</t>
+  </si>
+  <si>
+    <t>/ecf-cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CaseAugmentation/ojb-cit-ext:CaseParticipant/ojb-cit-ext:EntityPerson[@s:id=/ecf-cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ecf-cit:CitationSubject/nc:RoleOfPersonReference/@s:ref]/nc:PersonWeightMeasure/nc:MeasureUnitText</t>
+  </si>
+  <si>
+    <t>/ecf-cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CaseAugmentation/ojb-cit-ext:CaseParticipant/ojb-cit-ext:EntityPerson[@s:id=/ecf-cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ecf-cit:CitationSubject/nc:RoleOfPersonReference/@s:ref]/nc:PersonHairColorCode</t>
+  </si>
+  <si>
+    <t>/ecf-cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CaseAugmentation/ojb-cit-ext:CaseParticipant/ojb-cit-ext:EntityPerson[@s:id=/ecf-cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ecf-cit:CitationSubject/nc:RoleOfPersonReference/@s:ref]/nc:PersonEyeColorCode</t>
+  </si>
+  <si>
+    <t>/ecf-cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ojb-cit-ext:Vehicle[@s:id=/ecf-cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ojb-cit-ext:DrivingIncident/nc:IncidentVehicleAssociation/nc:ConveyanceReference/@s:ref]/nc:VehicleIdentification/nc:IdentificationID</t>
+  </si>
+  <si>
+    <t>/ecf-cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ojb-cit-ext:Vehicle[@s:id=/ecf-cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ojb-cit-ext:DrivingIncident/nc:IncidentVehicleAssociation/nc:ConveyanceReference/@s:ref]/nc:ConveyanceRegistrationPlateIdentification/nc:IdentificationID</t>
+  </si>
+  <si>
+    <t>/ecf-cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ojb-cit-ext:Vehicle[@s:id=/ecf-cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ojb-cit-ext:DrivingIncident/nc:IncidentVehicleAssociation/nc:ConveyanceReference/@s:ref]/nc:ConveyanceRegistrationPlateIdentification/j:IdentificationJurisdictionNCICLISCode</t>
+  </si>
+  <si>
+    <t>/ecf-cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ojb-cit-ext:Vehicle[@s:id=/ecf-cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ojb-cit-ext:DrivingIncident/nc:IncidentVehicleAssociation/nc:ConveyanceReference/@s:ref]/nc:ItemModelYearDate</t>
+  </si>
+  <si>
+    <t>/ecf-cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ojb-cit-ext:Vehicle[@s:id=/ecf-cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ojb-cit-ext:DrivingIncident/nc:IncidentVehicleAssociation/nc:ConveyanceReference/@s:ref]/nc:VehicleMakeCode</t>
+  </si>
+  <si>
+    <t>/ecf-cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ojb-cit-ext:Vehicle[@s:id=/ecf-cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ojb-cit-ext:DrivingIncident/nc:IncidentVehicleAssociation/nc:ConveyanceReference/@s:ref]/nc:VehicleColorPrimaryCode</t>
+  </si>
+  <si>
+    <t>/ecf-cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ojb-cit-ext:Vehicle[@s:id=/ecf-cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ojb-cit-ext:DrivingIncident/nc:IncidentVehicleAssociation/nc:ConveyanceReference/@s:ref]/nc:VehicleStyleCode</t>
+  </si>
+  <si>
+    <t>/ecf-cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ojb-cit-ext:Vehicle[@s:id=/ecf-cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ojb-cit-ext:DrivingIncident/nc:IncidentVehicleAssociation/nc:ConveyanceReference/@s:ref]/nc:VehicleCMVIndicator</t>
+  </si>
+  <si>
+    <t>/ecf-cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ojb-cit-ext:Vehicle[@s:id=/ecf-cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ojb-cit-ext:DrivingIncident/nc:IncidentVehicleAssociation/nc:ConveyanceReference/@s:ref]/ojb-cit-ext:VehicleAugmentation/ojb-cit-ext:VehicleHazardousMaterialIndicator</t>
+  </si>
+  <si>
+    <t>/ecf-cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ojb-cit-ext:DrivingIncident[@s:id=/ecf-cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ojb-cit-ext:DrivingIncident/nc:IncidentVehicleAssociation/nc:ActivityReference/@s:ref]/nc:ActivityIdentification/nc:IdentificationID</t>
+  </si>
+  <si>
+    <t>/ecf-cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ojb-cit-ext:DrivingIncident[@s:id=/ecf-cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ojb-cit-ext:DrivingIncident/nc:IncidentVehicleAssociation/nc:ActivityReference/@s:ref]/nc:ActivityDate/nc:DateTime</t>
+  </si>
+  <si>
+    <t>/ecf-cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ojb-cit-ext:DrivingIncident[@s:id=/ecf-cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ojb-cit-ext:DrivingIncident/nc:IncidentVehicleAssociation/nc:ActivityReference/@s:ref]/nc:IncidentLocation/nc:LocationAddress/nc:StructuredAddress/nc:LocationCityName</t>
+  </si>
+  <si>
+    <t>/ecf-cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ojb-cit-ext:DrivingIncident[@s:id=/ecf-cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ojb-cit-ext:DrivingIncident/nc:IncidentVehicleAssociation/nc:ActivityReference/@s:ref]/nc:IncidentLocation/nc:LocationHighway/nc:HighwayID</t>
+  </si>
+  <si>
+    <t>/ecf-cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ojb-cit-ext:DrivingIncident[@s:id=/ecf-cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ojb-cit-ext:DrivingIncident/nc:IncidentVehicleAssociation/nc:ActivityReference/@s:ref]/nc:IncidentLocation/nc:LocationHighway/nc:HighwayPositionText</t>
+  </si>
+  <si>
+    <t>/ecf-cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ojb-cit-ext:DrivingIncident[@s:id=/ecf-cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ojb-cit-ext:DrivingIncident/nc:IncidentVehicleAssociation/nc:ActivityReference/@s:ref]/nc:ActivityDescriptionText</t>
+  </si>
+  <si>
+    <t>/ecf-cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ecf-cit:CitationSubject/ecf-cit:PersonBloodAlcoholNumber</t>
+  </si>
+  <si>
+    <t>/ecf-cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ojb-cit-ext:DrivingIncident[@s:id=/ecf-cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ojb-cit-ext:DrivingIncident/nc:IncidentVehicleAssociation/nc:ActivityReference/@s:ref]/j:DrivingIncidentRecordedSpeedRate/nc:MeasureText</t>
+  </si>
+  <si>
+    <t>/ecf-cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ojb-cit-ext:DrivingIncident[@s:id=/ecf-cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ojb-cit-ext:DrivingIncident/nc:IncidentVehicleAssociation/nc:ActivityReference/@s:ref]/j:DrivingIncidentRecordedSpeedRate/nc:MeasureUnitText</t>
+  </si>
+  <si>
+    <t>/ecf-cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ojb-cit-ext:DrivingIncident[@s:id=/ecf-cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ojb-cit-ext:DrivingIncident/nc:IncidentVehicleAssociation/nc:ActivityReference/@s:ref]/j:DrivingIncidentLegalSpeedRate/nc:MeasureText</t>
+  </si>
+  <si>
+    <t>/ecf-cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ojb-cit-ext:DrivingIncident[@s:id=/ecf-cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ojb-cit-ext:DrivingIncident/nc:IncidentVehicleAssociation/nc:ActivityReference/@s:ref]/j:DrivingIncidentLegalSpeedRate/nc:MeasureUnitText</t>
+  </si>
+  <si>
+    <t>/ecf-cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ojb-cit-ext:DrivingIncident[@s:id=/ecf-cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ojb-cit-ext:DrivingIncident/nc:IncidentVehicleAssociation/nc:ActivityReference/@s:ref]/j:IncidentAugmentation/j:IncidentTrafficAccidentInvolvedIndicator</t>
+  </si>
+  <si>
+    <t>/ecf-cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ojb-cit-ext:DrivingIncident[@s:id=/ecf-cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ojb-cit-ext:DrivingIncident/nc:IncidentVehicleAssociation/nc:ActivityReference/@s:ref]/ojb-cit-ext:DrivingIncidentAugmentation/ojb-cit-ext:DrivingAccidentFatalityIndicator</t>
+  </si>
+  <si>
+    <t>/ecf-cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ojb-cit-ext:DrivingIncident[@s:id=/ecf-cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ojb-cit-ext:DrivingIncident/nc:IncidentVehicleAssociation/nc:ActivityReference/@s:ref]/ojb-cit-ext:DrivingIncidentAugmentation/ojb-cit-ext:SeatBeltViolationIndicator</t>
+  </si>
+  <si>
+    <t>/ecf-cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ojb-cit-ext:DrivingIncident[@s:id=/ecf-cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ojb-cit-ext:DrivingIncident/nc:IncidentVehicleAssociation/nc:ActivityReference/@s:ref]/ojb-cit-ext:DrivingIncidentAugmentation/ojb-cit-ext:CityReliefActIndicator</t>
+  </si>
+  <si>
+    <t>/ecf-cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ojb-cit-ext:DrivingIncident[@s:id=/ecf-cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ojb-cit-ext:DrivingIncident/nc:IncidentVehicleAssociation/nc:ActivityReference/@s:ref]/ojb-cit-ext:DrivingIncidentAugmentation/ojb-cit-ext:CityReliefActJuvenileIndicator</t>
+  </si>
+  <si>
+    <t>/ecf-cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ojb-cit-ext:DrivingIncident[@s:id=/ecf-cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ojb-cit-ext:DrivingIncident/nc:IncidentVehicleAssociation/nc:ActivityReference/@s:ref]/ojb-cit-ext:DrivingIncidentAugmentation/ojb-cit-ext:CityReliefActOtherIndicator</t>
+  </si>
+  <si>
+    <t>/ecf-cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ojb-cit-ext:DrivingIncident[@s:id=/ecf-cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ojb-cit-ext:DrivingIncident/nc:IncidentVehicleAssociation/nc:ActivityReference/@s:ref]/ojb-cit-ext:DrivingIncidentAugmentation/ojb-cit-ext:CityReliefActOtherText</t>
+  </si>
+  <si>
+    <t>/ecf-cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ojb-cit-ext:Offense/j:Statute/j:StatuteCodeIdentification/nc:IdentificationID</t>
+  </si>
+  <si>
+    <t>/ecf-cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ojb-cit-ext:Offense/ojb-cit-ext:OffenseViolatedStatute/j:StatuteCodeIdentification/nc:IdentificationID</t>
+  </si>
+  <si>
+    <t>/ecf-cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ojb-cit-ext:Offense/ojb-cit-ext:CFRStatute/j:StatuteCodeIdentification/nc:IdentificationID</t>
+  </si>
+  <si>
+    <t>/ecf-cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/j:CaseCharge/j:ChargeStatute/j:StatuteOffenseIdentification/nc:IdentificationID</t>
+  </si>
+  <si>
+    <t>/ecf-cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ojb-cit-ext:Offense/ojb-cit-ext:RelatedCriminalChargeIndicator</t>
+  </si>
+  <si>
+    <t>/ecf-cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ojb-cit-ext:Offense/ojb-cit-ext:DrivingOffensePoints</t>
+  </si>
+  <si>
+    <t>/ecf-cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ojb-cit-ext:Offense/ojb-cit-ext:OffenseFineAmountMinimum</t>
+  </si>
+  <si>
+    <t>/ecf-cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ojb-cit-ext:Offense/ojb-cit-ext:OffenseFineAmountMaximum</t>
+  </si>
+  <si>
+    <t>/ecf-cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CaseAugmentation/ojb-cit-ext:CaseParticipant/ecf:EntityPerson[@s:id=/ecf-cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ojb-cit-ext:Citation/j:CitationIssuingOfficial/nc:RoleOfPersonReference/@s:ref]/nc:PersonName/nc:PersonFullName</t>
+  </si>
+  <si>
+    <t>/ecf-cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ojb-cit-ext:Citation/j:CitationIssuingOfficial/j:EnforcementOfficialBadgeIdentification/nc:IdentificationID</t>
+  </si>
+  <si>
+    <t>/ecf-cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ojb-cit-ext:Citation/j:CitationAgency/nc:OrganizationPrimaryContactInformation/nc:ContactEntity/ecf:EntityOrganization/j:OrganizationAugmentation/j:OrganizationORIIdentification/nc:IdentificationID</t>
+  </si>
+  <si>
+    <t>/ecf-cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ojb-cit-ext:Citation/j:CitationAgency/nc:OrganizationName</t>
+  </si>
+  <si>
+    <t>/ecf-cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CaseAugmentation/ojb-cit-ext:CaseParticipant/ecf:EntityPerson[@s:id=/ecf-cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/nc:ImmediateFamilyAssociation/nc:PersonParentReference/@s:ref]/nc:PersonName/nc:PersonGivenName</t>
+  </si>
+  <si>
+    <t>/ecf-cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CaseAugmentation/ojb-cit-ext:CaseParticipant/ecf:EntityPerson[@s:id=/ecf-cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/nc:ImmediateFamilyAssociation/nc:PersonParentReference/@s:ref]/nc:PersonName/nc:PersonSurName</t>
+  </si>
+  <si>
+    <t>/ecf-cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CaseAugmentation/ojb-cit-ext:CaseParticipant/ecf:EntityPerson[@s:id=/ecf-cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/nc:ImmediateFamilyAssociation/nc:PersonParentReference/@s:ref]/ecf:PersonAugmentation/nc:ContactInformation/nc:ContactMailingAddress/nc:StructuredAddress/nc:LocationStreet/nc:StreetFullText</t>
+  </si>
+  <si>
+    <t>/ecf-cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CaseAugmentation/ojb-cit-ext:CaseParticipant/ecf:EntityPerson[@s:id=/ecf-cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/nc:ImmediateFamilyAssociation/nc:PersonParentReference/@s:ref]/ecf:PersonAugmentation/nc:ContactInformation/nc:ContactMailingAddress/nc:StructuredAddress/nc:LocationCityName</t>
+  </si>
+  <si>
+    <t>/ecf-cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CaseAugmentation/ojb-cit-ext:CaseParticipant/ecf:EntityPerson[@s:id=/ecf-cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/nc:ImmediateFamilyAssociation/nc:PersonParentReference/@s:ref]/ecf:PersonAugmentation/nc:ContactInformation/nc:ContactMailingAddress/nc:StructuredAddress/nc:LocationCountryFIPS10-4Code</t>
+  </si>
+  <si>
+    <t>/ecf-cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CaseAugmentation/ojb-cit-ext:CaseParticipant/ecf:EntityPerson[@s:id=/ecf-cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/nc:ImmediateFamilyAssociation/nc:PersonParentReference/@s:ref]/ecf:PersonAugmentation/nc:ContactInformation/nc:ContactMailingAddress/nc:StructuredAddress/nc:LocationPostalCode</t>
+  </si>
+  <si>
+    <t>/ecf-cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CaseAugmentation/ojb-cit-ext:CaseParticipant/ojb-cit-ext:EntityPerson[@s:id=/ecf-cfm:CoreFilingMessage/ojb-cit-doc:CitationCase/ojb-cit-ext:CitationCaseAugmentation/ecf-cit:CitationSubject/nc:RoleOfPersonReference/@s:ref]/ojb-cit-ext:PersonAugmentation/ojb-cit-ext:PersonDriverLicense/ojb-cit-ext:DriverLicenseCDLIndicator</t>
   </si>
 </sst>
 </file>
@@ -2904,9 +2904,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E87"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E87" sqref="E87"/>
+      <selection pane="bottomLeft" activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -2934,7 +2934,7 @@
         <v>123</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>284</v>
+        <v>210</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="19" customHeight="1">
@@ -2960,7 +2960,7 @@
         <v>82734800</v>
       </c>
       <c r="E3" s="15" t="s">
-        <v>209</v>
+        <v>212</v>
       </c>
     </row>
     <row r="4" spans="1:5" s="3" customFormat="1">
@@ -2977,7 +2977,7 @@
         <v>42304</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>210</v>
+        <v>213</v>
       </c>
     </row>
     <row r="5" spans="1:5" s="3" customFormat="1" ht="28">
@@ -2994,7 +2994,7 @@
         <v>105</v>
       </c>
       <c r="E5" s="8" t="s">
-        <v>211</v>
+        <v>214</v>
       </c>
     </row>
     <row r="6" spans="1:5" s="3" customFormat="1" ht="28">
@@ -3011,7 +3011,7 @@
         <v>1</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>212</v>
+        <v>215</v>
       </c>
     </row>
     <row r="7" spans="1:5" s="3" customFormat="1" ht="28">
@@ -3028,7 +3028,7 @@
         <v>0</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>213</v>
+        <v>216</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -3051,7 +3051,7 @@
         <v>163</v>
       </c>
       <c r="E9" s="15" t="s">
-        <v>214</v>
+        <v>217</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -3074,7 +3074,7 @@
         <v>206</v>
       </c>
       <c r="E11" s="15" t="s">
-        <v>215</v>
+        <v>218</v>
       </c>
     </row>
     <row r="12" spans="1:5">
@@ -3100,7 +3100,7 @@
         <v>126</v>
       </c>
       <c r="E13" s="15" t="s">
-        <v>216</v>
+        <v>219</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="42">
@@ -3117,7 +3117,7 @@
         <v>127</v>
       </c>
       <c r="E14" s="15" t="s">
-        <v>217</v>
+        <v>220</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="42">
@@ -3134,7 +3134,7 @@
         <v>128</v>
       </c>
       <c r="E15" s="15" t="s">
-        <v>218</v>
+        <v>221</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="56">
@@ -3151,7 +3151,7 @@
         <v>129</v>
       </c>
       <c r="E16" s="15" t="s">
-        <v>230</v>
+        <v>222</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="42">
@@ -3168,7 +3168,7 @@
         <v>130</v>
       </c>
       <c r="E17" s="15" t="s">
-        <v>231</v>
+        <v>223</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="56">
@@ -3185,7 +3185,7 @@
         <v>124</v>
       </c>
       <c r="E18" s="15" t="s">
-        <v>232</v>
+        <v>224</v>
       </c>
     </row>
     <row r="19" spans="1:5" s="3" customFormat="1" ht="42">
@@ -3202,7 +3202,7 @@
         <v>131</v>
       </c>
       <c r="E19" s="15" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="42">
@@ -3219,7 +3219,7 @@
         <v>41444812</v>
       </c>
       <c r="E20" s="15" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="42">
@@ -3236,7 +3236,7 @@
         <v>124</v>
       </c>
       <c r="E21" s="15" t="s">
-        <v>233</v>
+        <v>227</v>
       </c>
     </row>
     <row r="22" spans="1:5" ht="42">
@@ -3253,7 +3253,7 @@
         <v>12345678</v>
       </c>
       <c r="E22" s="15" t="s">
-        <v>244</v>
+        <v>228</v>
       </c>
     </row>
     <row r="23" spans="1:5" s="3" customFormat="1" ht="84">
@@ -3270,7 +3270,7 @@
         <v>8023631111</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>282</v>
+        <v>229</v>
       </c>
     </row>
     <row r="24" spans="1:5" s="3" customFormat="1" ht="84">
@@ -3287,7 +3287,7 @@
         <v>8023631112</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>283</v>
+        <v>230</v>
       </c>
     </row>
     <row r="25" spans="1:5" s="3" customFormat="1" ht="42">
@@ -3304,7 +3304,7 @@
         <v>24014</v>
       </c>
       <c r="E25" s="15" t="s">
-        <v>221</v>
+        <v>231</v>
       </c>
     </row>
     <row r="26" spans="1:5" s="3" customFormat="1" ht="42">
@@ -3321,7 +3321,7 @@
         <v>132</v>
       </c>
       <c r="E26" s="15" t="s">
-        <v>220</v>
+        <v>232</v>
       </c>
     </row>
     <row r="27" spans="1:5" s="3" customFormat="1" ht="56">
@@ -3338,7 +3338,7 @@
         <v>133</v>
       </c>
       <c r="E27" s="15" t="s">
-        <v>219</v>
+        <v>233</v>
       </c>
     </row>
     <row r="28" spans="1:5" s="3" customFormat="1" ht="42">
@@ -3355,7 +3355,7 @@
         <v>134</v>
       </c>
       <c r="E28" s="15" t="s">
-        <v>222</v>
+        <v>234</v>
       </c>
     </row>
     <row r="29" spans="1:5" s="3" customFormat="1" ht="42">
@@ -3366,7 +3366,7 @@
         <v>170</v>
       </c>
       <c r="E29" s="15" t="s">
-        <v>223</v>
+        <v>235</v>
       </c>
     </row>
     <row r="30" spans="1:5" s="3" customFormat="1" ht="42">
@@ -3383,7 +3383,7 @@
         <v>135</v>
       </c>
       <c r="E30" s="15" t="s">
-        <v>225</v>
+        <v>236</v>
       </c>
     </row>
     <row r="31" spans="1:5" s="3" customFormat="1" ht="42">
@@ -3394,7 +3394,7 @@
         <v>171</v>
       </c>
       <c r="E31" s="15" t="s">
-        <v>224</v>
+        <v>237</v>
       </c>
     </row>
     <row r="32" spans="1:5" s="3" customFormat="1" ht="42">
@@ -3411,7 +3411,7 @@
         <v>135</v>
       </c>
       <c r="E32" s="15" t="s">
-        <v>226</v>
+        <v>238</v>
       </c>
     </row>
     <row r="33" spans="1:5" s="3" customFormat="1" ht="42">
@@ -3428,7 +3428,7 @@
         <v>135</v>
       </c>
       <c r="E33" s="15" t="s">
-        <v>227</v>
+        <v>239</v>
       </c>
     </row>
     <row r="34" spans="1:5">
@@ -3454,7 +3454,7 @@
         <v>167</v>
       </c>
       <c r="E35" s="3" t="s">
-        <v>235</v>
+        <v>240</v>
       </c>
     </row>
     <row r="36" spans="1:5" s="3" customFormat="1" ht="56">
@@ -3468,7 +3468,7 @@
         <v>136</v>
       </c>
       <c r="E36" s="3" t="s">
-        <v>236</v>
+        <v>241</v>
       </c>
     </row>
     <row r="37" spans="1:5" s="3" customFormat="1" ht="56">
@@ -3485,7 +3485,7 @@
         <v>124</v>
       </c>
       <c r="E37" s="3" t="s">
-        <v>237</v>
+        <v>242</v>
       </c>
     </row>
     <row r="38" spans="1:5" s="3" customFormat="1" ht="42">
@@ -3502,7 +3502,7 @@
         <v>2015</v>
       </c>
       <c r="E38" s="3" t="s">
-        <v>238</v>
+        <v>243</v>
       </c>
     </row>
     <row r="39" spans="1:5" s="3" customFormat="1" ht="42">
@@ -3519,7 +3519,7 @@
         <v>138</v>
       </c>
       <c r="E39" s="3" t="s">
-        <v>239</v>
+        <v>244</v>
       </c>
     </row>
     <row r="40" spans="1:5" s="3" customFormat="1" ht="42">
@@ -3536,7 +3536,7 @@
         <v>139</v>
       </c>
       <c r="E40" s="3" t="s">
-        <v>240</v>
+        <v>245</v>
       </c>
     </row>
     <row r="41" spans="1:5" s="3" customFormat="1" ht="42">
@@ -3553,7 +3553,7 @@
         <v>140</v>
       </c>
       <c r="E41" s="3" t="s">
-        <v>241</v>
+        <v>246</v>
       </c>
     </row>
     <row r="42" spans="1:5" s="3" customFormat="1" ht="42">
@@ -3570,7 +3570,7 @@
         <v>0</v>
       </c>
       <c r="E42" s="3" t="s">
-        <v>242</v>
+        <v>247</v>
       </c>
     </row>
     <row r="43" spans="1:5" s="3" customFormat="1" ht="42">
@@ -3587,7 +3587,7 @@
         <v>0</v>
       </c>
       <c r="E43" s="3" t="s">
-        <v>243</v>
+        <v>248</v>
       </c>
     </row>
     <row r="44" spans="1:5">
@@ -3613,7 +3613,7 @@
         <v>125</v>
       </c>
       <c r="E45" s="2" t="s">
-        <v>245</v>
+        <v>249</v>
       </c>
     </row>
     <row r="46" spans="1:5" s="3" customFormat="1" ht="42">
@@ -3630,7 +3630,7 @@
         <v>141</v>
       </c>
       <c r="E46" s="15" t="s">
-        <v>246</v>
+        <v>250</v>
       </c>
     </row>
     <row r="47" spans="1:5" s="3" customFormat="1" ht="56">
@@ -3644,7 +3644,7 @@
         <v>28</v>
       </c>
       <c r="E47" s="15" t="s">
-        <v>247</v>
+        <v>251</v>
       </c>
     </row>
     <row r="48" spans="1:5" s="3" customFormat="1" ht="56">
@@ -3661,7 +3661,7 @@
         <v>143</v>
       </c>
       <c r="E48" s="15" t="s">
-        <v>248</v>
+        <v>252</v>
       </c>
     </row>
     <row r="49" spans="1:5" s="3" customFormat="1" ht="56">
@@ -3678,7 +3678,7 @@
         <v>144</v>
       </c>
       <c r="E49" s="15" t="s">
-        <v>249</v>
+        <v>253</v>
       </c>
     </row>
     <row r="50" spans="1:5" s="3" customFormat="1" ht="42">
@@ -3695,7 +3695,7 @@
         <v>145</v>
       </c>
       <c r="E50" s="15" t="s">
-        <v>250</v>
+        <v>254</v>
       </c>
     </row>
     <row r="51" spans="1:5" s="3" customFormat="1">
@@ -3712,7 +3712,7 @@
         <v>0.2</v>
       </c>
       <c r="E51" s="15" t="s">
-        <v>251</v>
+        <v>255</v>
       </c>
     </row>
     <row r="52" spans="1:5" s="3" customFormat="1" ht="56">
@@ -3729,7 +3729,7 @@
         <v>30</v>
       </c>
       <c r="E52" s="15" t="s">
-        <v>252</v>
+        <v>256</v>
       </c>
     </row>
     <row r="53" spans="1:5" s="3" customFormat="1" ht="56">
@@ -3743,7 +3743,7 @@
         <v>169</v>
       </c>
       <c r="E53" s="15" t="s">
-        <v>253</v>
+        <v>257</v>
       </c>
     </row>
     <row r="54" spans="1:5" s="3" customFormat="1" ht="42">
@@ -3760,7 +3760,7 @@
         <v>40</v>
       </c>
       <c r="E54" s="15" t="s">
-        <v>254</v>
+        <v>258</v>
       </c>
     </row>
     <row r="55" spans="1:5" s="3" customFormat="1" ht="56">
@@ -3774,7 +3774,7 @@
         <v>169</v>
       </c>
       <c r="E55" s="15" t="s">
-        <v>255</v>
+        <v>259</v>
       </c>
     </row>
     <row r="56" spans="1:5" s="3" customFormat="1" ht="56">
@@ -3791,7 +3791,7 @@
         <v>0</v>
       </c>
       <c r="E56" s="15" t="s">
-        <v>257</v>
+        <v>260</v>
       </c>
     </row>
     <row r="57" spans="1:5" s="3" customFormat="1" ht="42">
@@ -3808,7 +3808,7 @@
         <v>0</v>
       </c>
       <c r="E57" s="15" t="s">
-        <v>256</v>
+        <v>261</v>
       </c>
     </row>
     <row r="58" spans="1:5" s="3" customFormat="1" ht="42">
@@ -3825,7 +3825,7 @@
         <v>0</v>
       </c>
       <c r="E58" s="15" t="s">
-        <v>258</v>
+        <v>262</v>
       </c>
     </row>
     <row r="59" spans="1:5" ht="42">
@@ -3842,7 +3842,7 @@
         <v>1</v>
       </c>
       <c r="E59" s="15" t="s">
-        <v>259</v>
+        <v>263</v>
       </c>
     </row>
     <row r="60" spans="1:5" ht="42">
@@ -3859,7 +3859,7 @@
         <v>1</v>
       </c>
       <c r="E60" s="15" t="s">
-        <v>260</v>
+        <v>264</v>
       </c>
     </row>
     <row r="61" spans="1:5" ht="42">
@@ -3876,7 +3876,7 @@
         <v>1</v>
       </c>
       <c r="E61" s="15" t="s">
-        <v>261</v>
+        <v>265</v>
       </c>
     </row>
     <row r="62" spans="1:5" ht="42">
@@ -3890,7 +3890,7 @@
         <v>88</v>
       </c>
       <c r="E62" s="15" t="s">
-        <v>262</v>
+        <v>266</v>
       </c>
     </row>
     <row r="63" spans="1:5">
@@ -3916,7 +3916,7 @@
         <v>147</v>
       </c>
       <c r="E64" s="3" t="s">
-        <v>274</v>
+        <v>267</v>
       </c>
     </row>
     <row r="65" spans="1:5" s="3" customFormat="1" ht="28">
@@ -3933,7 +3933,7 @@
         <v>146</v>
       </c>
       <c r="E65" s="3" t="s">
-        <v>275</v>
+        <v>268</v>
       </c>
     </row>
     <row r="66" spans="1:5" s="3" customFormat="1" ht="28">
@@ -3950,7 +3950,7 @@
         <v>148</v>
       </c>
       <c r="E66" s="3" t="s">
-        <v>276</v>
+        <v>269</v>
       </c>
     </row>
     <row r="67" spans="1:5" s="3" customFormat="1" ht="28">
@@ -3967,7 +3967,7 @@
         <v>149</v>
       </c>
       <c r="E67" s="3" t="s">
-        <v>277</v>
+        <v>270</v>
       </c>
     </row>
     <row r="68" spans="1:5" s="3" customFormat="1">
@@ -3984,7 +3984,7 @@
         <v>0</v>
       </c>
       <c r="E68" s="3" t="s">
-        <v>278</v>
+        <v>271</v>
       </c>
     </row>
     <row r="69" spans="1:5" s="3" customFormat="1">
@@ -4001,7 +4001,7 @@
         <v>2</v>
       </c>
       <c r="E69" s="3" t="s">
-        <v>279</v>
+        <v>272</v>
       </c>
     </row>
     <row r="70" spans="1:5" s="3" customFormat="1">
@@ -4018,7 +4018,7 @@
         <v>47</v>
       </c>
       <c r="E70" s="8" t="s">
-        <v>280</v>
+        <v>273</v>
       </c>
     </row>
     <row r="71" spans="1:5" s="3" customFormat="1">
@@ -4035,7 +4035,7 @@
         <v>1197</v>
       </c>
       <c r="E71" s="8" t="s">
-        <v>281</v>
+        <v>274</v>
       </c>
     </row>
     <row r="72" spans="1:5">
@@ -4061,7 +4061,7 @@
         <v>150</v>
       </c>
       <c r="E73" s="3" t="s">
-        <v>263</v>
+        <v>275</v>
       </c>
     </row>
     <row r="74" spans="1:5" s="3" customFormat="1" ht="28">
@@ -4078,7 +4078,7 @@
         <v>12345</v>
       </c>
       <c r="E74" s="3" t="s">
-        <v>265</v>
+        <v>276</v>
       </c>
     </row>
     <row r="75" spans="1:5" s="3" customFormat="1">
@@ -4092,7 +4092,7 @@
         <v>53</v>
       </c>
       <c r="E75" s="2" t="s">
-        <v>264</v>
+        <v>209</v>
       </c>
     </row>
     <row r="76" spans="1:5" s="3" customFormat="1" ht="42">
@@ -4109,7 +4109,7 @@
         <v>151</v>
       </c>
       <c r="E76" s="3" t="s">
-        <v>267</v>
+        <v>277</v>
       </c>
     </row>
     <row r="77" spans="1:5" s="3" customFormat="1">
@@ -4126,7 +4126,7 @@
         <v>152</v>
       </c>
       <c r="E77" s="3" t="s">
-        <v>266</v>
+        <v>278</v>
       </c>
     </row>
     <row r="78" spans="1:5">
@@ -4152,7 +4152,7 @@
         <v>153</v>
       </c>
       <c r="E79" s="3" t="s">
-        <v>268</v>
+        <v>279</v>
       </c>
     </row>
     <row r="80" spans="1:5" ht="28">
@@ -4169,7 +4169,7 @@
         <v>126</v>
       </c>
       <c r="E80" s="3" t="s">
-        <v>269</v>
+        <v>280</v>
       </c>
     </row>
     <row r="81" spans="1:5" ht="42">
@@ -4186,7 +4186,7 @@
         <v>154</v>
       </c>
       <c r="E81" s="3" t="s">
-        <v>270</v>
+        <v>281</v>
       </c>
     </row>
     <row r="82" spans="1:5" ht="42">
@@ -4203,7 +4203,7 @@
         <v>155</v>
       </c>
       <c r="E82" s="3" t="s">
-        <v>271</v>
+        <v>282</v>
       </c>
     </row>
     <row r="83" spans="1:5" ht="42">
@@ -4220,7 +4220,7 @@
         <v>124</v>
       </c>
       <c r="E83" s="3" t="s">
-        <v>272</v>
+        <v>283</v>
       </c>
     </row>
     <row r="84" spans="1:5" ht="42">
@@ -4237,7 +4237,7 @@
         <v>156</v>
       </c>
       <c r="E84" s="3" t="s">
-        <v>273</v>
+        <v>284</v>
       </c>
     </row>
     <row r="85" spans="1:5">
@@ -4263,12 +4263,12 @@
         <v>0</v>
       </c>
       <c r="E86" s="15" t="s">
-        <v>234</v>
+        <v>285</v>
       </c>
     </row>
     <row r="87" spans="1:5" ht="119" customHeight="1">
       <c r="A87" s="17" t="s">
-        <v>285</v>
+        <v>211</v>
       </c>
       <c r="B87" s="18"/>
       <c r="C87" s="18"/>

</xml_diff>